<commit_message>
Subida de pdf al sistema
</commit_message>
<xml_diff>
--- a/Entregables/Cuadro comparativo de proveedores.xlsx
+++ b/Entregables/Cuadro comparativo de proveedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto_Py\Cetaf_Python_Uikit_V1\Entregables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BCEBC1-55E6-4B1A-A7C2-3D649635DE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D03EDC-601C-4358-ACC5-634189A8E20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
     <t>Sistema Operativo</t>
   </si>
   <si>
-    <t>Ubuntu Server</t>
+    <t>CentOS</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -231,26 +231,20 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -263,7 +257,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -554,184 +554,184 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>3565000</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>1890000</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>1948000</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>3021000</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>9997000</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>8945000</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>7078000</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="4">
         <v>6113000</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>3332100</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>4675000</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <v>2913000</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="4">
         <v>2319000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C7" s="9"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <f>MIN(C4,C5,C6,E4,E5,E6,G4,G5,G6,I4,I5,I6)</f>
         <v>1890000</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <f>AVERAGE(C4,C5,C6,E4,E5,E6,G4,G5,G6,I4,I5,I6)</f>
         <v>4649675</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <f>MAX(C4,C6,C5,E4,E5,E6,G4,G5,G6,I4,I5,I6)</f>
         <v>9997000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">

</xml_diff>